<commit_message>
Edited plan and renamed a testclass
</commit_message>
<xml_diff>
--- a/Documentation/Plan.xlsx
+++ b/Documentation/Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JonathanLydemann\source\repos\MicrowaveHandin\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89202722-4FC2-4B04-A524-401A428978EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109F586F-E0E6-4FDC-9D14-7CAD6CC7571F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1401,7 +1401,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
@@ -1574,10 +1574,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>

</xml_diff>